<commit_message>
[ISP-2] Configurazione forecast per Intesa
</commit_message>
<xml_diff>
--- a/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/05_EntityType_intesa.xlsx
+++ b/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/05_EntityType_intesa.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="863" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="863" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -3227,11 +3227,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:D152"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -3255,7 +3254,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>102</v>
       </c>
@@ -3269,7 +3268,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>102</v>
       </c>
@@ -3283,7 +3282,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>102</v>
       </c>
@@ -3297,7 +3296,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>102</v>
       </c>
@@ -3311,7 +3310,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>102</v>
       </c>
@@ -3325,7 +3324,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>102</v>
       </c>
@@ -3339,7 +3338,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>102</v>
       </c>
@@ -3353,7 +3352,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
@@ -3367,7 +3366,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>102</v>
       </c>
@@ -3381,7 +3380,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>102</v>
       </c>
@@ -3395,7 +3394,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="12" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>102</v>
       </c>
@@ -3409,7 +3408,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -3423,7 +3422,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
@@ -3437,7 +3436,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>102</v>
       </c>
@@ -3451,7 +3450,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>102</v>
       </c>
@@ -3465,7 +3464,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>102</v>
       </c>
@@ -3479,7 +3478,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>102</v>
       </c>
@@ -3493,7 +3492,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>102</v>
       </c>
@@ -3507,7 +3506,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>102</v>
       </c>
@@ -3521,7 +3520,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>102</v>
       </c>
@@ -3535,7 +3534,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>102</v>
       </c>
@@ -3549,7 +3548,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>102</v>
       </c>
@@ -3563,7 +3562,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>102</v>
       </c>
@@ -3577,7 +3576,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
@@ -3591,7 +3590,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>102</v>
       </c>
@@ -3605,7 +3604,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>102</v>
       </c>
@@ -3619,7 +3618,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>102</v>
       </c>
@@ -3633,7 +3632,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>102</v>
       </c>
@@ -3647,7 +3646,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>102</v>
       </c>
@@ -3661,7 +3660,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>102</v>
       </c>
@@ -3675,7 +3674,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>102</v>
       </c>
@@ -3689,7 +3688,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>102</v>
       </c>
@@ -3703,7 +3702,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>102</v>
       </c>
@@ -3717,7 +3716,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>102</v>
       </c>
@@ -3731,7 +3730,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>102</v>
       </c>
@@ -3745,7 +3744,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>102</v>
       </c>
@@ -3759,7 +3758,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>102</v>
       </c>
@@ -3773,7 +3772,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>102</v>
       </c>
@@ -3787,7 +3786,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>102</v>
       </c>
@@ -3801,7 +3800,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>102</v>
       </c>
@@ -3815,7 +3814,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>102</v>
       </c>
@@ -3829,7 +3828,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>102</v>
       </c>
@@ -3843,7 +3842,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>102</v>
       </c>
@@ -3857,7 +3856,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>102</v>
       </c>
@@ -3871,7 +3870,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>102</v>
       </c>
@@ -3885,7 +3884,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>102</v>
       </c>
@@ -3899,7 +3898,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>102</v>
       </c>
@@ -3913,7 +3912,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>102</v>
       </c>
@@ -3927,7 +3926,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>102</v>
       </c>
@@ -3941,7 +3940,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>102</v>
       </c>
@@ -3955,7 +3954,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
@@ -3969,7 +3968,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>102</v>
       </c>
@@ -3983,7 +3982,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>102</v>
       </c>
@@ -3997,7 +3996,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>102</v>
       </c>
@@ -4011,7 +4010,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>102</v>
       </c>
@@ -4025,7 +4024,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>210</v>
       </c>
@@ -4039,7 +4038,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>210</v>
       </c>
@@ -4053,7 +4052,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>210</v>
       </c>
@@ -4067,7 +4066,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>210</v>
       </c>
@@ -4081,7 +4080,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>210</v>
       </c>
@@ -4095,7 +4094,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>210</v>
       </c>
@@ -4109,7 +4108,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>210</v>
       </c>
@@ -4123,7 +4122,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>210</v>
       </c>
@@ -4137,7 +4136,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>101</v>
       </c>
@@ -4151,7 +4150,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>101</v>
       </c>
@@ -4165,7 +4164,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>101</v>
       </c>
@@ -4179,7 +4178,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>101</v>
       </c>
@@ -4193,7 +4192,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -4207,7 +4206,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>101</v>
       </c>
@@ -4221,7 +4220,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>101</v>
       </c>
@@ -4235,7 +4234,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="65" t="s">
         <v>98</v>
       </c>
@@ -4249,7 +4248,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="65" t="s">
         <v>98</v>
       </c>
@@ -4263,7 +4262,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="65" t="s">
         <v>98</v>
       </c>
@@ -4277,7 +4276,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="65" t="s">
         <v>99</v>
       </c>
@@ -4291,7 +4290,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="65" t="s">
         <v>99</v>
       </c>
@@ -4305,7 +4304,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="65" t="s">
         <v>99</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="65" t="s">
         <v>99</v>
       </c>
@@ -4333,7 +4332,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>272</v>
       </c>
@@ -4347,7 +4346,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>272</v>
       </c>
@@ -4361,7 +4360,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>272</v>
       </c>
@@ -4375,7 +4374,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>272</v>
       </c>
@@ -4389,7 +4388,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>272</v>
       </c>
@@ -4403,7 +4402,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>272</v>
       </c>
@@ -4417,7 +4416,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>272</v>
       </c>
@@ -4431,7 +4430,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>272</v>
       </c>
@@ -4445,7 +4444,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>272</v>
       </c>
@@ -4459,7 +4458,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>272</v>
       </c>
@@ -4473,7 +4472,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>272</v>
       </c>
@@ -4487,7 +4486,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>272</v>
       </c>
@@ -4501,7 +4500,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>272</v>
       </c>
@@ -4515,7 +4514,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>272</v>
       </c>
@@ -4529,7 +4528,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>272</v>
       </c>
@@ -4543,7 +4542,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>272</v>
       </c>
@@ -4557,7 +4556,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>272</v>
       </c>
@@ -4571,7 +4570,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>272</v>
       </c>
@@ -4585,7 +4584,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="97" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>102</v>
       </c>
@@ -4599,7 +4598,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="98" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>102</v>
       </c>
@@ -4613,7 +4612,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="99" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>102</v>
       </c>
@@ -4641,7 +4640,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="101" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>102</v>
       </c>
@@ -4655,7 +4654,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="102" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>102</v>
       </c>
@@ -4669,7 +4668,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="103" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>102</v>
       </c>
@@ -4697,7 +4696,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="105" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>210</v>
       </c>
@@ -4711,7 +4710,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="106" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>210</v>
       </c>
@@ -4725,7 +4724,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="107" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>210</v>
       </c>
@@ -4753,7 +4752,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="109" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>102</v>
       </c>
@@ -4767,7 +4766,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="110" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>102</v>
       </c>
@@ -4781,7 +4780,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="111" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>102</v>
       </c>
@@ -4795,7 +4794,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="112" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>102</v>
       </c>
@@ -4809,7 +4808,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="113" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>102</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="114" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>102</v>
       </c>
@@ -4837,7 +4836,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="115" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>102</v>
       </c>
@@ -4851,7 +4850,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="116" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>102</v>
       </c>
@@ -4865,7 +4864,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>102</v>
       </c>
@@ -4879,7 +4878,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="118" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>102</v>
       </c>
@@ -4893,7 +4892,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="119" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>272</v>
       </c>
@@ -4907,7 +4906,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="120" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>102</v>
       </c>
@@ -4921,7 +4920,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="121" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>102</v>
       </c>
@@ -4935,7 +4934,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="122" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>102</v>
       </c>
@@ -4963,7 +4962,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="124" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>210</v>
       </c>
@@ -4977,7 +4976,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="125" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>210</v>
       </c>
@@ -4991,7 +4990,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="126" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>210</v>
       </c>
@@ -5005,7 +5004,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="127" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>210</v>
       </c>
@@ -5019,7 +5018,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="128" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>210</v>
       </c>
@@ -5033,7 +5032,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="129" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>102</v>
       </c>
@@ -5047,7 +5046,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="130" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>102</v>
       </c>
@@ -5061,7 +5060,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="131" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>102</v>
       </c>
@@ -5075,7 +5074,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="132" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>102</v>
       </c>
@@ -5089,7 +5088,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="133" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>210</v>
       </c>
@@ -5103,7 +5102,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="134" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>102</v>
       </c>
@@ -5117,7 +5116,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="135" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>102</v>
       </c>
@@ -5131,7 +5130,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="136" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>102</v>
       </c>
@@ -5145,7 +5144,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="137" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>102</v>
       </c>
@@ -5159,7 +5158,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="138" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>102</v>
       </c>
@@ -5173,7 +5172,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="139" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="s">
         <v>102</v>
       </c>
@@ -5187,7 +5186,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="140" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="s">
         <v>102</v>
       </c>
@@ -5201,7 +5200,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="141" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="s">
         <v>210</v>
       </c>
@@ -5215,7 +5214,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="142" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="s">
         <v>210</v>
       </c>
@@ -5229,7 +5228,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="143" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="s">
         <v>210</v>
       </c>
@@ -5243,7 +5242,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="144" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="s">
         <v>210</v>
       </c>
@@ -5257,7 +5256,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="145" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="s">
         <v>210</v>
       </c>
@@ -5271,7 +5270,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="146" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="s">
         <v>210</v>
       </c>
@@ -5285,7 +5284,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="147" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
         <v>102</v>
       </c>
@@ -5299,7 +5298,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="148" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="s">
         <v>102</v>
       </c>
@@ -5313,7 +5312,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="149" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149" s="1" t="s">
         <v>102</v>
       </c>
@@ -5327,7 +5326,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="150" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150" s="1" t="s">
         <v>102</v>
       </c>
@@ -5341,7 +5340,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="151" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151" s="1" t="s">
         <v>102</v>
       </c>
@@ -5355,7 +5354,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="152" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152" s="1" t="s">
         <v>102</v>
       </c>
@@ -5370,15 +5369,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D152">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="IMP_TOT_PREL_RIPROP_Mix"/>
-        <filter val="IMP_TOT_PRELEVATO_Mix"/>
-        <filter val="IMP_TOT_VERSAMENTO_Mix"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>